<commit_message>
Entrega da parte GQA -1 e 2 e RAP 6 até 10
</commit_message>
<xml_diff>
--- a/Gerência de Qualidade/Planilha GQA.xlsx
+++ b/Gerência de Qualidade/Planilha GQA.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jean\Documents\UFG\4Semestre\Processo de Software\Trabalho-Execução\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josimar\Documents\GitHub\Trabalho-processo-software-pratica-parte2\Gerência de Qualidade\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="987" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7905" tabRatio="987" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instruções para preenchimento" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="53">
   <si>
     <t>INSTRUÇÕES</t>
   </si>
@@ -188,13 +188,22 @@
   </si>
   <si>
     <t>Documento de Definição de Processo de Garantia de Qualidade</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -315,8 +324,16 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -353,6 +370,24 @@
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="27">
     <border>
@@ -709,7 +744,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -894,6 +929,21 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="16" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1660,8 +1710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z110"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1800,7 +1850,7 @@
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
     </row>
-    <row r="5" spans="1:26" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
         <v>39</v>
       </c>
@@ -1874,7 +1924,7 @@
         <f>HYPERLINK("https://github.com/gilmarfilho/ProcessoDeSoftware/blob/master/TEMPLATES/TEMPLATES%20GQA/Medi%C3%A7%C3%B5es%20de%20controle%20de%20qualidade.docx","X")</f>
         <v>X</v>
       </c>
-      <c r="D7" s="66" t="s">
+      <c r="D7" s="67" t="s">
         <v>36</v>
       </c>
       <c r="E7" s="25"/>
@@ -1987,7 +2037,7 @@
     <row r="11" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="28"/>
       <c r="B11" s="29" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="C11" s="30"/>
       <c r="D11" s="30"/>
@@ -2053,7 +2103,7 @@
         <f>HYPERLINK("https://github.com/gilmarfilho/ProcessoDeSoftware/blob/master/TEMPLATES/TEMPLATES%20GQA/Documento%20de%20auditoria%20de%20qualidade.docx","X")</f>
         <v>X</v>
       </c>
-      <c r="D13" s="66" t="s">
+      <c r="D13" s="69" t="s">
         <v>36</v>
       </c>
       <c r="E13" s="25"/>
@@ -2194,7 +2244,7 @@
     <row r="18" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="28"/>
       <c r="B18" s="29" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="C18" s="30"/>
       <c r="D18" s="30"/>
@@ -3900,7 +3950,7 @@
         <f>HYPERLINK("https://github.com/gilmarfilho/ProcessoDeSoftware/blob/master/TEMPLATES/TEMPLATES%20GPR/Plano%20de%20Recursos%20Humanos.docx","X")</f>
         <v>X</v>
       </c>
-      <c r="D75" s="66" t="s">
+      <c r="D75" s="68" t="s">
         <v>36</v>
       </c>
       <c r="E75" s="25"/>
@@ -4041,7 +4091,7 @@
     <row r="80" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="24"/>
       <c r="B80" s="29" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="C80" s="30"/>
       <c r="D80" s="30"/>
@@ -4107,7 +4157,7 @@
         <f>HYPERLINK("https://github.com/gilmarfilho/ProcessoDeSoftware/blob/master/Documento%20de%20Defini%C3%A7%C3%A3o%20de%20Processo%20de%20Garantia%20de%20Qualidade.docx","X")</f>
         <v>X</v>
       </c>
-      <c r="D82" s="52" t="str">
+      <c r="D82" s="70" t="str">
         <f>HYPERLINK("https://github.com/gilmarfilho/ProcessoDeSoftware/blob/master/Documento%20de%20Defini%C3%A7%C3%A3o%20de%20Processo%20de%20Garantia%20de%20Qualidade.docx","X")</f>
         <v>X</v>
       </c>
@@ -4249,7 +4299,7 @@
     <row r="87" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="24"/>
       <c r="B87" s="29" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="C87" s="30"/>
       <c r="D87" s="30"/>
@@ -4315,7 +4365,7 @@
         <f>HYPERLINK("https://github.com/gilmarfilho/ProcessoDeSoftware/blob/master/Documento%20de%20Defini%C3%A7%C3%A3o%20de%20Processo%20de%20Garantia%20de%20Qualidade.docx","X")</f>
         <v>X</v>
       </c>
-      <c r="D89" s="52" t="str">
+      <c r="D89" s="71" t="str">
         <f>HYPERLINK("https://github.com/gilmarfilho/ProcessoDeSoftware/blob/master/Documento%20de%20Defini%C3%A7%C3%A3o%20de%20Processo%20de%20Garantia%20de%20Qualidade.docx","X")</f>
         <v>X</v>
       </c>
@@ -4457,7 +4507,7 @@
     <row r="94" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="24"/>
       <c r="B94" s="29" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="C94" s="30"/>
       <c r="D94" s="30"/>
@@ -4523,7 +4573,7 @@
         <f>HYPERLINK("https://github.com/gilmarfilho/ProcessoDeSoftware/blob/master/TEMPLATES/TEMPLATES%20GQA/Documento%20de%20auditoria%20de%20qualidade.docx","X")</f>
         <v>X</v>
       </c>
-      <c r="D96" s="66" t="s">
+      <c r="D96" s="69" t="s">
         <v>36</v>
       </c>
       <c r="E96" s="25"/>
@@ -4664,7 +4714,7 @@
     <row r="101" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="24"/>
       <c r="B101" s="29" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="C101" s="30"/>
       <c r="D101" s="30"/>
@@ -4730,7 +4780,7 @@
         <f>HYPERLINK("https://github.com/gilmarfilho/ProcessoDeSoftware/blob/master/TEMPLATES/TEMPLATES%20GQA/Documento%20de%20acompanhamento%20de%20n%C3%A3o-conformidades.docx","X")</f>
         <v>X</v>
       </c>
-      <c r="D103" s="66" t="s">
+      <c r="D103" s="69" t="s">
         <v>36</v>
       </c>
       <c r="E103" s="25"/>
@@ -4871,7 +4921,7 @@
     <row r="108" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="24"/>
       <c r="B108" s="29" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="C108" s="30"/>
       <c r="D108" s="30"/>
@@ -4917,6 +4967,6 @@
     <hyperlink ref="D28" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>